<commit_message>
[PHOENIX-5849] Modified the data according to the production dump
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="76">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">contractor</t>
   </si>
   <si>
-    <t xml:space="preserve">G Basheer Ahmed</t>
+    <t xml:space="preserve">KMC001</t>
   </si>
   <si>
     <t xml:space="preserve">voucher2</t>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">budgetCheckWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1301001</t>
   </si>
   <si>
     <t xml:space="preserve">voucherWithOutSubledger</t>
@@ -289,7 +292,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -319,6 +322,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,7 +372,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,6 +386,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,29 +412,29 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="52.6222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="58.0111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -738,7 +751,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>34</v>
@@ -749,7 +762,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>27</v>
@@ -766,8 +779,8 @@
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
+      <c r="G8" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>34</v>
@@ -778,7 +791,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -842,15 +855,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="D:D C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.0592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="88.4888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -858,32 +871,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -904,22 +917,22 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D:D H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -936,27 +949,27 @@
         <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>19</v>
@@ -965,10 +978,10 @@
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
@@ -1004,21 +1017,21 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="D:D B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.4481481481482"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.6666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="47.5259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.1518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.8814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.4259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1026,36 +1039,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
@@ -1067,19 +1080,19 @@
         <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>100</v>
@@ -1103,25 +1116,25 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="D:D E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.5518518518518"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.11481481481482"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.8074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.8962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="42.8222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1129,22 +1142,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1153,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -1167,7 +1180,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -1179,13 +1192,13 @@
         <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>2101001</v>

</xml_diff>

<commit_message>
[PHOENIX-6110] Modified the data in excel reader
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -152,34 +152,43 @@
     <t xml:space="preserve">budgetCheckWithSubledger</t>
   </si>
   <si>
+    <t xml:space="preserve">2202105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3501003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remittance</t>
+  </si>
+  <si>
     <t xml:space="preserve">2101001</t>
   </si>
   <si>
-    <t xml:space="preserve">3501003</t>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheckWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1301001</t>
   </si>
   <si>
     <t xml:space="preserve">ENGINEERING</t>
   </si>
   <si>
     <t xml:space="preserve">Water Supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remittance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">budgetCheckWithOutSubledger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1301001</t>
   </si>
   <si>
     <t xml:space="preserve">voucherWithOutSubledger</t>
@@ -292,7 +301,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -322,12 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,7 +375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -386,10 +389,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,29 +411,29 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="58.0111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="59.4814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -689,13 +688,13 @@
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>33</v>
@@ -722,7 +721,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>25</v>
@@ -733,7 +732,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>27</v>
@@ -751,18 +750,18 @@
         <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>27</v>
@@ -779,19 +778,19 @@
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>41</v>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -860,10 +859,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="88.4888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.2407407407408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="90.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -871,32 +870,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -923,16 +922,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -949,27 +948,27 @@
         <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>19</v>
@@ -978,10 +977,10 @@
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
@@ -1023,15 +1022,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.1518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.8814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.4222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.6444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.4259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.0555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="53.7"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1039,60 +1038,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>100</v>
@@ -1122,19 +1121,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="42.8222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.0925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.9"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1142,22 +1141,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1166,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -1180,25 +1179,25 @@
     </row>
     <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>2101001</v>

</xml_diff>

<commit_message>
[PHOENIX-6110] Modified the finance data in excel reader
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/financialTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -140,105 +140,99 @@
     <t xml:space="preserve">Expense</t>
   </si>
   <si>
+    <t xml:space="preserve">2202105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherBillPayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheckWithSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3501003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheckWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1301001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherWithSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bankName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDHRA BANK-Andhra Bank RTC Busstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4502110--110710100009664--ANDHRA BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDHRA BANK Andhra Bank RTC Busstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billSubType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountCodeDebit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountCodeCredit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expenseDebitAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expenseCreditAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expenseNetAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expenseBill</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUBLIC HEALTH AND SANITATION</t>
   </si>
   <si>
-    <t xml:space="preserve">Public Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voucherBillPayment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">budgetCheckWithSubledger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2202105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3501003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General Administration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remittance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2101001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">budgetCheckWithOutSubledger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1301001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voucherWithOutSubledger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voucherWithSubledger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bankName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDHRA BANK-Andhra Bank RTC Busstand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4502110--110710100009664--ANDHRA BANK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBI1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDHRA BANK Andhra Bank RTC Busstand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billSubType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountCodeDebit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountCodeCredit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expenseDebitAmount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expenseCreditAmount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expenseNetAmount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expenseBill</t>
-  </si>
-  <si>
     <t xml:space="preserve">3100</t>
   </si>
   <si>
@@ -291,6 +285,9 @@
   </si>
   <si>
     <t xml:space="preserve">directBankDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1201005</t>
   </si>
 </sst>
 </file>
@@ -301,7 +298,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -331,6 +328,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,6 +392,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,29 +418,29 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="59.4814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.2962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="60.9518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -546,8 +553,8 @@
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>2101001</v>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>21</v>
@@ -558,11 +565,11 @@
       <c r="G3" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>100</v>
@@ -585,7 +592,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>27</v>
@@ -593,8 +600,8 @@
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>2101001</v>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
@@ -605,11 +612,11 @@
       <c r="G4" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>100</v>
@@ -632,7 +639,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>27</v>
@@ -641,7 +648,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -653,10 +660,10 @@
         <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L5" s="1" t="n">
         <v>100</v>
@@ -679,7 +686,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>27</v>
@@ -687,23 +694,23 @@
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>3502002</v>
@@ -721,7 +728,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>25</v>
@@ -732,7 +739,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>27</v>
@@ -750,18 +757,18 @@
         <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>27</v>
@@ -779,18 +786,18 @@
         <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -798,8 +805,8 @@
       <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>2101001</v>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
@@ -810,11 +817,11 @@
       <c r="G9" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>100</v>
@@ -859,10 +866,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.2407407407408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="90.7407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.0037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="92.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -870,32 +877,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -922,16 +929,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -948,39 +955,39 @@
         <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
@@ -1022,15 +1029,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.6444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.4259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.0555555555556"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="53.7"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.7222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.7"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.2333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="55.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1038,60 +1045,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>100</v>
@@ -1116,24 +1123,24 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.2555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.0925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.9"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.3333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="44.9777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1141,22 +1148,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1165,7 +1172,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
@@ -1179,34 +1186,34 @@
     </row>
     <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>2101001</v>
+        <v>48</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>2101001</v>
+      <c r="J2" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>24</v>

</xml_diff>